<commit_message>
"signin and logout from excel data"
</commit_message>
<xml_diff>
--- a/src/com/trainee/aizaz/selenium/Tests/TestDataForSignIn.xlsx
+++ b/src/com/trainee/aizaz/selenium/Tests/TestDataForSignIn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajaz/Documents/training-automation/src/com/trainee/aizaz/selenium/Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{8C2017A5-2D8C-A040-9870-E1475DEC25AF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{030EF25C-05B5-2A4D-9298-D885E7A755E9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16220" xr2:uid="{0286BC9C-0A6D-9949-91E2-23887B55638F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" xr2:uid="{0286BC9C-0A6D-9949-91E2-23887B55638F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,40 +25,62 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>aizaz</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>hello</t>
   </si>
   <si>
-    <t>hi</t>
-  </si>
-  <si>
-    <t>alan</t>
-  </si>
-  <si>
-    <t>bye</t>
+    <t>aizaz1@gmail.com</t>
+  </si>
+  <si>
+    <t>aizaz2@gmail.com</t>
+  </si>
+  <si>
+    <t>aizaz3@gmail.com</t>
+  </si>
+  <si>
+    <t>aizaz4@gmail.com</t>
+  </si>
+  <si>
+    <t>aizaz5@gmail.com</t>
+  </si>
+  <si>
+    <t>Anjali225*</t>
+  </si>
+  <si>
+    <t>geetanjaliguda1998@gmail.com</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,13 +100,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,47 +423,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF1E095-B5C6-B14F-9265-1C134C86D853}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{38A375C2-B60D-9F44-926E-914CB23B0371}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{68049F28-9AA0-3346-8E2F-E9C8CFB1E0DF}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{15C0AA0A-8E0C-D448-8EF8-FA56FA7FCC7B}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{BA61C70C-817F-7741-8CA0-8E7FF7B852A0}"/>
+    <hyperlink ref="A2" r:id="rId5" xr:uid="{5F33D31C-8806-0D4A-ABFC-101BBB4B7291}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{29A7C7BD-90D7-3E41-956C-3DAFE772AB55}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>